<commit_message>
Complex properties in tables state that they are not round trippable
This was always the case, but now you get a nice warning message,
and the tests won't attempt to write out to excel. Before the
there was no warning, and the tests would attempt to write to excel
but would raise an exception.
</commit_message>
<xml_diff>
--- a/Test/TestExcelFiles/ComplexObjectWithinTable/ComplexObjectWithinTable.xlsx
+++ b/Test/TestExcelFiles/ComplexObjectWithinTable/ComplexObjectWithinTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\Test\TestExcelFiles\ComplexObjectWithinTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0D6BD0F6-33CB-47F3-83C8-274AF5B08CE7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DB694421-166D-4526-99C3-0C9CD234C25B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
   </bookViews>
@@ -69,9 +69,6 @@
     <t>A warning should be issued to this effect</t>
   </si>
   <si>
-    <t>AnyTableProperty of</t>
-  </si>
-  <si>
     <t>AnyTable</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>ComplexObjectType</t>
+  </si>
+  <si>
+    <t>AnyTableProperty table of</t>
   </si>
 </sst>
 </file>
@@ -540,7 +540,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,10 +582,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -595,12 +595,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>